<commit_message>
feat: add molde/rotura hours to informe excel and local preview script
</commit_message>
<xml_diff>
--- a/app/templates/Template_Informe.xlsx
+++ b/app/templates/Template_Informe.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\crmnew\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\crmnew\api-geofal-crm\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A03D5A1-B695-4765-96A6-E56B748968E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A703E820-9E9D-4551-A065-1D036FB0ACD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{930961E3-46E8-4944-A657-321E9D043D38}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <author>HP</author>
   </authors>
   <commentList>
-    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{DC7211CB-86A1-4E50-B91C-87E4909D0F93}">
+    <comment ref="H16" authorId="0" shapeId="0" xr:uid="{DC7211CB-86A1-4E50-B91C-87E4909D0F93}">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -147,7 +147,10 @@
     <t>Densidad</t>
   </si>
   <si>
-    <t>ESTO DATOS VIENEN FORMATO RECEPCION</t>
+    <t>Hora moldeo</t>
+  </si>
+  <si>
+    <t>Hora rotura</t>
   </si>
 </sst>
 </file>
@@ -157,7 +160,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000\-&quot;CO-26&quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,11 +200,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <vertAlign val="superscript"/>
       <sz val="8"/>
@@ -209,7 +207,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,14 +220,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -285,36 +277,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -322,7 +290,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -333,48 +300,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D18AB54-13F3-4496-B406-2D49A32253B9}">
-  <dimension ref="A5:J24"/>
+  <dimension ref="A5:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,138 +663,133 @@
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="19"/>
       <c r="I5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="20"/>
       <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="20"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="18"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="I12" s="12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I13" s="16" t="s">
+      <c r="A13" s="9"/>
+      <c r="I13" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="15" spans="1:10" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+    </row>
+    <row r="16" spans="1:10" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J16" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="10"/>
-    </row>
     <row r="17" spans="1:10" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="10"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="15"/>
     </row>
     <row r="18" spans="1:10" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="10"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>22</v>
-      </c>
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="1:10" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>